<commit_message>
Add possible endings to the goals document
</commit_message>
<xml_diff>
--- a/PowerSpel-PenTest/Overzicht_goals.xlsx
+++ b/PowerSpel-PenTest/Overzicht_goals.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="49">
   <si>
     <t>Penetraties</t>
   </si>
@@ -115,6 +115,57 @@
   </si>
   <si>
     <t>Maximaal behaalbare punten:</t>
+  </si>
+  <si>
+    <t>Van terrein aflopen</t>
+  </si>
+  <si>
+    <t>Nooduitgang bovenste verdieping gebruiken</t>
+  </si>
+  <si>
+    <t>091100</t>
+  </si>
+  <si>
+    <t>070704</t>
+  </si>
+  <si>
+    <t>060704</t>
+  </si>
+  <si>
+    <t>070802</t>
+  </si>
+  <si>
+    <t>Kopieerapparaat misbruiken</t>
+  </si>
+  <si>
+    <t>SSD-pc gebruiken</t>
+  </si>
+  <si>
+    <t>IA-pc gebruiken</t>
+  </si>
+  <si>
+    <t>Personeelsdossiers inzien</t>
+  </si>
+  <si>
+    <t>Herrie maken in loods</t>
+  </si>
+  <si>
+    <t>Sleutelbeen breken op serverruimtedeur</t>
+  </si>
+  <si>
+    <t>040600</t>
+  </si>
+  <si>
+    <t>060900</t>
+  </si>
+  <si>
+    <t>050802</t>
+  </si>
+  <si>
+    <t>070401</t>
+  </si>
+  <si>
+    <t>Airco saboteren</t>
   </si>
 </sst>
 </file>
@@ -451,7 +502,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -491,6 +542,33 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -775,12 +853,12 @@
   <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
@@ -971,64 +1049,118 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="5"/>
+      <c r="A17" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="25">
+        <v>1</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="7"/>
+      <c r="A18" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="27">
+        <v>2</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="7"/>
+      <c r="A19" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="27">
+        <v>3</v>
+      </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="7"/>
+      <c r="A20" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="27">
+        <v>4</v>
+      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="7"/>
+      <c r="A21" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="31" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" s="27">
+        <v>4</v>
+      </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="7"/>
+      <c r="A22" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="27">
+        <v>4</v>
+      </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="7"/>
+      <c r="A23" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="27">
+        <v>4</v>
+      </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="7"/>
+      <c r="A24" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="27">
+        <v>5</v>
+      </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="6"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="7"/>
+      <c r="A25" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" s="27">
+        <v>6</v>
+      </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="7"/>
+      <c r="A26" s="26"/>
+      <c r="B26" s="31"/>
+      <c r="C26" s="27"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="6"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="7"/>
+      <c r="A27" s="26"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="27"/>
     </row>
     <row r="28" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="8"/>
-      <c r="B28" s="9"/>
-      <c r="C28" s="10"/>
+      <c r="A28" s="28"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="29"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>